<commit_message>
add tugas 1 > import user
</commit_message>
<xml_diff>
--- a/Minggu8/Jobsheet 8/public/template_barang.xlsx
+++ b/Minggu8/Jobsheet 8/public/template_barang.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\PWL_2025\Minggu8\Jobsheet 8\public\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ANGELINA\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{304D3B0B-6A4F-4CF0-89F2-62A7AC4F7586}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C284BC4D-8B28-4E2D-89DD-1D1A7BCFC800}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8835" yWindow="0" windowWidth="9900" windowHeight="10920" xr2:uid="{27DBCC50-F3BF-45DF-AD9E-4AC4FB617F7E}"/>
+    <workbookView xWindow="9510" yWindow="0" windowWidth="9780" windowHeight="11370" xr2:uid="{BDAA3379-DFDD-41F0-A96D-80987CEB74E0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,10 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>kategori_id</t>
   </si>
@@ -48,46 +51,34 @@
     <t>harga_jual</t>
   </si>
   <si>
-    <t>Telur Omega (10 butir)</t>
-  </si>
-  <si>
-    <t>Sari Roti</t>
-  </si>
-  <si>
-    <t>Shampoo Pantene</t>
-  </si>
-  <si>
-    <t>Baju Bayi 2th</t>
-  </si>
-  <si>
-    <t>Cleo 600ml</t>
-  </si>
-  <si>
-    <t>KTG003</t>
-  </si>
-  <si>
-    <t>KTG009</t>
-  </si>
-  <si>
-    <t>KTG002</t>
-  </si>
-  <si>
-    <t>KTG004</t>
-  </si>
-  <si>
-    <t>BRG017</t>
-  </si>
-  <si>
-    <t>BRG018</t>
-  </si>
-  <si>
-    <t>BRG019</t>
-  </si>
-  <si>
-    <t>BRG020</t>
-  </si>
-  <si>
-    <t>BRG021</t>
+    <t>M003</t>
+  </si>
+  <si>
+    <t>M004</t>
+  </si>
+  <si>
+    <t>B003</t>
+  </si>
+  <si>
+    <t>B004</t>
+  </si>
+  <si>
+    <t>H003</t>
+  </si>
+  <si>
+    <t>Liptint Velvel</t>
+  </si>
+  <si>
+    <t>BB Creaam</t>
+  </si>
+  <si>
+    <t>Body Lotion Bengkoang</t>
+  </si>
+  <si>
+    <t>Shower Gel Bunga</t>
+  </si>
+  <si>
+    <t>Shampoo Anti Rontok</t>
   </si>
 </sst>
 </file>
@@ -103,7 +94,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="8"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -131,7 +123,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -445,127 +437,128 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8636A15-CFD3-4D3D-8424-D6B73A0A8590}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5316837-A43D-4BD6-92D1-318D93705A26}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" customWidth="1"/>
-    <col min="3" max="3" width="21.7109375" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" customWidth="1"/>
+    <col min="1" max="1" width="9.26953125" customWidth="1"/>
+    <col min="2" max="2" width="13.54296875" customWidth="1"/>
+    <col min="3" max="3" width="22.6328125" customWidth="1"/>
+    <col min="4" max="4" width="10.81640625" customWidth="1"/>
+    <col min="5" max="5" width="10.453125" customWidth="1"/>
+    <col min="6" max="6" width="10.6328125" customWidth="1"/>
+    <col min="7" max="7" width="11.08984375" customWidth="1"/>
+    <col min="8" max="8" width="11.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2">
+        <v>35000</v>
+      </c>
+      <c r="E2">
+        <v>55000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3">
+        <v>65000</v>
+      </c>
+      <c r="E3">
+        <v>80000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4">
+        <v>28000</v>
+      </c>
+      <c r="E4">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5">
+        <v>45000</v>
+      </c>
+      <c r="E5">
+        <v>65000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2">
-        <v>22000</v>
-      </c>
-      <c r="E2">
-        <v>25000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3">
-        <v>11500</v>
-      </c>
-      <c r="E3">
-        <v>12500</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4">
-        <v>17500</v>
-      </c>
-      <c r="E4">
-        <v>18500</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5">
-        <v>89000</v>
-      </c>
-      <c r="E5">
-        <v>92500</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" t="s">
-        <v>9</v>
-      </c>
       <c r="D6">
-        <v>3750</v>
+        <v>37000</v>
       </c>
       <c r="E6">
-        <v>4300</v>
+        <v>50000</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>